<commit_message>
votes add summary&result, property add trust type
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/林世嘉_2013-07-15_財產申報表_tmpf70f1.xlsx
+++ b/legislator/property/output/normal/林世嘉_2013-07-15_財產申報表_tmpf70f1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -103,9 +103,6 @@
     <t>買賣</t>
   </si>
   <si>
-    <t>1III：!貝買</t>
-  </si>
-  <si>
     <t>(超過五年）</t>
   </si>
   <si>
@@ -145,12 +142,6 @@
     <t>3分之1</t>
   </si>
   <si>
-    <t>I"rl"T广貝買</t>
-  </si>
-  <si>
-    <t>riftr:貝買</t>
-  </si>
-  <si>
     <t>building</t>
   </si>
   <si>
@@ -160,7 +151,13 @@
     <t>福斯PASSAT2.0</t>
   </si>
   <si>
+    <t>福斯PASSAT2.0TDI</t>
+  </si>
+  <si>
     <t>94年01月28日</t>
+  </si>
+  <si>
+    <t>民國102年6月</t>
   </si>
   <si>
     <t>car</t>
@@ -649,16 +646,16 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>22</v>
@@ -667,7 +664,7 @@
         <v>1740</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2" s="2">
         <v>15</v>
@@ -699,19 +696,19 @@
         <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="I3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>22</v>
@@ -720,7 +717,7 @@
         <v>1740</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" s="2">
         <v>16</v>
@@ -755,16 +752,16 @@
         <v>27</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>22</v>
@@ -773,7 +770,7 @@
         <v>1740</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O4" s="2">
         <v>17</v>
@@ -853,13 +850,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2">
         <v>83.23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
@@ -871,16 +868,16 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>22</v>
@@ -889,7 +886,7 @@
         <v>1740</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2" s="2">
         <v>22</v>
@@ -906,13 +903,13 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2">
         <v>337.9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
@@ -921,19 +918,19 @@
         <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>22</v>
@@ -942,7 +939,7 @@
         <v>1740</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" s="2">
         <v>23</v>
@@ -959,13 +956,13 @@
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2">
         <v>26.56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -977,16 +974,16 @@
         <v>27</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>22</v>
@@ -995,7 +992,7 @@
         <v>1740</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O4" s="2">
         <v>24</v>
@@ -1012,13 +1009,13 @@
         <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2">
         <v>211.47</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>23</v>
@@ -1027,19 +1024,19 @@
         <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>22</v>
@@ -1048,7 +1045,7 @@
         <v>1740</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O5" s="2">
         <v>25</v>
@@ -1067,7 +1064,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1078,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1119,7 +1116,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>1984</v>
@@ -1128,22 +1125,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>22</v>
@@ -1152,10 +1149,54 @@
         <v>1740</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="2">
         <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1300000</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1740</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="2">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1173,10 +1214,10 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1214,34 +1255,34 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2">
         <v>5566788</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>22</v>
@@ -1250,42 +1291,42 @@
         <v>1740</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2">
         <v>6675465</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>22</v>
@@ -1294,42 +1335,42 @@
         <v>1740</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2">
         <v>10500000</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>22</v>
@@ -1338,42 +1379,42 @@
         <v>1740</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2">
         <v>2161265</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>22</v>
@@ -1382,42 +1423,42 @@
         <v>1740</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N5" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2">
         <v>563630</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>22</v>
@@ -1426,42 +1467,42 @@
         <v>1740</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" s="2">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="2">
         <v>543011</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>22</v>
@@ -1470,42 +1511,42 @@
         <v>1740</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" s="2">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="2">
         <v>714257</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>22</v>
@@ -1514,42 +1555,42 @@
         <v>1740</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2">
         <v>2000000</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="I9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>22</v>
@@ -1558,10 +1599,10 @@
         <v>1740</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N9" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>